<commit_message>
feat: Refactor Department pages, add Global Administration page, update Dean/HOD profiles, fix admissions data
</commit_message>
<xml_diff>
--- a/public/2025-26 Faculty Directory/B S & H25-26 FACULTY LIST  DINAL FROM dr yvrr.xlsx
+++ b/public/2025-26 Faculty Directory/B S & H25-26 FACULTY LIST  DINAL FROM dr yvrr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CSE_DEAN\Downloads\New folder (4)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CSE_DEAN\Desktop\nriit-generativeai-campus\public\2025-26 Faculty Directory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80D2B44F-7F51-4085-8B35-8458ADC20A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17661C8F-E709-45EE-B1A4-E5A134C730E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,8 @@
     <sheet name="PHYSICS" sheetId="3" state="hidden" r:id="rId10"/>
     <sheet name="MATHS" sheetId="2" state="hidden" r:id="rId11"/>
     <sheet name="S&amp;H 25-26 DR YVRR" sheetId="20" r:id="rId12"/>
-    <sheet name="DS 25-26_x0009__x0009__x0009__x0009__x0009__x0009_" sheetId="23" r:id="rId13"/>
-    <sheet name="consolidated list" sheetId="22" state="hidden" r:id="rId14"/>
+    <sheet name="consolidated list" sheetId="22" state="hidden" r:id="rId13"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId15"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'S&amp;H 25-26 DR YVRR'!$F$1:$F$76</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TOTAL!$B$1:$B$84</definedName>
@@ -1263,76 +1259,6 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
-          <xdr:row>39</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="4" name="Picture 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AD8FD28-C5A4-783F-B0ED-87C51548F26D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="'[1]DS 25-26'!$A$1:$G$36" spid="_x0000_s14339"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="8410575" cy="7600950"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1378,22 +1304,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="DS 25-26"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5497,7 +5407,7 @@
   <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F3"/>
+      <selection activeCell="A5" sqref="A5:XFD72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7415,22 +7325,6 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902BA0AF-8219-4D76-958D-E0F3F06193BC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76257A77-6C9A-46FF-9EB3-665A998D542F}">
   <dimension ref="B8:D19"/>
   <sheetViews>

</xml_diff>